<commit_message>
corrected rna number for rnaSample_hbrown_10.15.19
</commit_message>
<xml_diff>
--- a/s1cDNASample/s1CDNASample_hbrown_10.23.19.xlsx
+++ b/s1cDNASample/s1CDNASample_hbrown_10.23.19.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/Desktop/4a metadata sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/s1cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70C7EEC2-CDB0-AD47-A759-E45D4299A923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39991C4-A210-204B-B562-C952D781C17F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12860" yWindow="4300" windowWidth="20720" windowHeight="14920" xr2:uid="{5EC711FD-29FB-E046-A8C8-B789A9DE105B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="53">
   <si>
     <t>rnaDate</t>
   </si>
@@ -81,13 +81,121 @@
   </si>
   <si>
     <t>random</t>
+  </si>
+  <si>
+    <t>4a 1</t>
+  </si>
+  <si>
+    <t>4a 2</t>
+  </si>
+  <si>
+    <t>4a 3</t>
+  </si>
+  <si>
+    <t>4a 4</t>
+  </si>
+  <si>
+    <t>4a 5</t>
+  </si>
+  <si>
+    <t>4a 6</t>
+  </si>
+  <si>
+    <t>4a 7</t>
+  </si>
+  <si>
+    <t>4a 8</t>
+  </si>
+  <si>
+    <t>4a 9</t>
+  </si>
+  <si>
+    <t>4a 10</t>
+  </si>
+  <si>
+    <t>4a 11</t>
+  </si>
+  <si>
+    <t>4a 12</t>
+  </si>
+  <si>
+    <t>4a 13</t>
+  </si>
+  <si>
+    <t>4a 14</t>
+  </si>
+  <si>
+    <t>4a 15</t>
+  </si>
+  <si>
+    <t>4a 16</t>
+  </si>
+  <si>
+    <t>4a 17</t>
+  </si>
+  <si>
+    <t>4a 18</t>
+  </si>
+  <si>
+    <t>4a 19</t>
+  </si>
+  <si>
+    <t>4a 20</t>
+  </si>
+  <si>
+    <t>4a 21</t>
+  </si>
+  <si>
+    <t>4a 22</t>
+  </si>
+  <si>
+    <t>4a 23</t>
+  </si>
+  <si>
+    <t>4a 24</t>
+  </si>
+  <si>
+    <t>4a 25</t>
+  </si>
+  <si>
+    <t>4a 26</t>
+  </si>
+  <si>
+    <t>JR1 1</t>
+  </si>
+  <si>
+    <t>JR1 2</t>
+  </si>
+  <si>
+    <t>JR1 3</t>
+  </si>
+  <si>
+    <t>JR1 4</t>
+  </si>
+  <si>
+    <t>JR1 5</t>
+  </si>
+  <si>
+    <t>JR1 6</t>
+  </si>
+  <si>
+    <t>JR1 7</t>
+  </si>
+  <si>
+    <t>JR1 8</t>
+  </si>
+  <si>
+    <t>JR1 9</t>
+  </si>
+  <si>
+    <t>JR1 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,6 +212,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -127,10 +241,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B358D8B-1875-5D4D-9AC7-F17D5670928A}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,8 +625,8 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -556,8 +673,8 @@
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -588,8 +705,8 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>3</v>
+      <c r="C4" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -620,8 +737,8 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>4</v>
+      <c r="C5" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -652,8 +769,8 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>5</v>
+      <c r="C6" t="s">
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -684,8 +801,8 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
-        <v>6</v>
+      <c r="C7" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -716,8 +833,8 @@
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
-        <v>7</v>
+      <c r="C8" t="s">
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -748,8 +865,8 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>8</v>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -780,8 +897,8 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
-        <v>9</v>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -812,8 +929,8 @@
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
-        <v>10</v>
+      <c r="C11" t="s">
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -844,8 +961,8 @@
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>11</v>
+      <c r="C12" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -876,8 +993,8 @@
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
-        <v>12</v>
+      <c r="C13" t="s">
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -908,8 +1025,8 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14">
-        <v>13</v>
+      <c r="C14" t="s">
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -940,8 +1057,8 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15">
-        <v>14</v>
+      <c r="C15" t="s">
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -972,8 +1089,8 @@
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C16">
-        <v>15</v>
+      <c r="C16" t="s">
+        <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -1004,8 +1121,8 @@
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C17">
-        <v>16</v>
+      <c r="C17" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -1036,8 +1153,8 @@
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18">
-        <v>17</v>
+      <c r="C18" t="s">
+        <v>33</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -1068,8 +1185,8 @@
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19">
-        <v>18</v>
+      <c r="C19" t="s">
+        <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
@@ -1100,8 +1217,8 @@
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20">
-        <v>19</v>
+      <c r="C20" t="s">
+        <v>35</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1132,8 +1249,8 @@
       <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C21">
-        <v>20</v>
+      <c r="C21" t="s">
+        <v>36</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
@@ -1164,8 +1281,8 @@
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22">
-        <v>21</v>
+      <c r="C22" t="s">
+        <v>37</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
@@ -1196,8 +1313,8 @@
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C23">
-        <v>22</v>
+      <c r="C23" t="s">
+        <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1228,8 +1345,8 @@
       <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C24">
-        <v>23</v>
+      <c r="C24" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
@@ -1260,8 +1377,8 @@
       <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C25">
-        <v>24</v>
+      <c r="C25" t="s">
+        <v>40</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>12</v>
@@ -1292,8 +1409,8 @@
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C26">
-        <v>25</v>
+      <c r="C26" t="s">
+        <v>41</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>12</v>
@@ -1324,8 +1441,8 @@
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C27">
-        <v>26</v>
+      <c r="C27" t="s">
+        <v>42</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>12</v>
@@ -1356,8 +1473,8 @@
       <c r="B28" t="s">
         <v>11</v>
       </c>
-      <c r="C28">
-        <v>27</v>
+      <c r="C28" t="s">
+        <v>43</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -1388,8 +1505,8 @@
       <c r="B29" t="s">
         <v>11</v>
       </c>
-      <c r="C29">
-        <v>28</v>
+      <c r="C29" t="s">
+        <v>44</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -1420,8 +1537,8 @@
       <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="C30">
-        <v>29</v>
+      <c r="C30" t="s">
+        <v>45</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -1452,8 +1569,8 @@
       <c r="B31" t="s">
         <v>11</v>
       </c>
-      <c r="C31">
-        <v>30</v>
+      <c r="C31" t="s">
+        <v>46</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -1484,8 +1601,8 @@
       <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="C32">
-        <v>31</v>
+      <c r="C32" t="s">
+        <v>47</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -1516,8 +1633,8 @@
       <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="C33">
-        <v>32</v>
+      <c r="C33" t="s">
+        <v>48</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -1548,8 +1665,8 @@
       <c r="B34" t="s">
         <v>11</v>
       </c>
-      <c r="C34">
-        <v>33</v>
+      <c r="C34" t="s">
+        <v>49</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -1580,8 +1697,8 @@
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C35">
-        <v>34</v>
+      <c r="C35" t="s">
+        <v>50</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -1612,8 +1729,8 @@
       <c r="B36" t="s">
         <v>11</v>
       </c>
-      <c r="C36">
-        <v>35</v>
+      <c r="C36" t="s">
+        <v>51</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -1644,8 +1761,8 @@
       <c r="B37" t="s">
         <v>11</v>
       </c>
-      <c r="C37">
-        <v>36</v>
+      <c r="C37" t="s">
+        <v>52</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>

</xml_diff>